<commit_message>
made some changes in the Frontend
</commit_message>
<xml_diff>
--- a/diagrams/the material sizes.xlsx
+++ b/diagrams/the material sizes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\desktop D\3rd year\PUSL3190_MDCGunathilaka\diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764E7E58-7E85-48AE-B21A-D14968BDE76B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7450B0FD-8C60-4009-A74F-4E682D746DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -875,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6:I9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>